<commit_message>
MAJ résultats et évaluation prédiction
</commit_message>
<xml_diff>
--- a/SparkApplication/Résultats/Résultats.xlsx
+++ b/SparkApplication/Résultats/Résultats.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{43DFEA64-CA56-421B-B5AB-938A96105E38}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{519A9EFC-BB82-402A-B4A7-E73CAB5F4300}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1094,6 +1094,330 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'1 instance de calcul distante'!$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dataset "big"  (66Mo)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'1 instance de calcul distante'!$A$5:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'1 instance de calcul distante'!$E$5:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>4294</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13203</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14469</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23091</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41952</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65126</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>101389</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>110383</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>180195</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-75A1-48AD-AFD5-5BC767A24258}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1143412815"/>
+        <c:axId val="1138506191"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1143412815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1138506191"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1138506191"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1143412815"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -1789,7 +2113,331 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2 instances de calcul distantes'!$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dataset "big"  (66Mo)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'2 instances de calcul distantes'!$A$5:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'2 instances de calcul distantes'!$E$5:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>3957</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6472</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10180</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13701</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27685</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43774</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>53251</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>74125</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>114520</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3517-4BE8-871E-EA5D2680FF18}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1150739599"/>
+        <c:axId val="1138550255"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1150739599"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1138550255"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1138550255"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1150739599"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="fr-FR"/>
@@ -2499,6 +3147,330 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'3 instances de calcul distantes'!$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dataset "big"  (66Mo)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'3 instances de calcul distantes'!$A$5:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'3 instances de calcul distantes'!$E$5:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2873</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5671</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8628</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11076</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16788</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21548</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28521</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31452</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>44576</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>98473</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-99A0-484F-9681-8B908DEF1F4F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1150713391"/>
+        <c:axId val="1151278591"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1150713391"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1151278591"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1151278591"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1150713391"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2619,6 +3591,126 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3626,6 +4718,1515 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4161,6 +6762,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BA58E9F-6E61-4448-BB03-02EA78C794BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4207,6 +6844,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B85E239-555E-4F21-A2C5-3E028BF6F528}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4248,6 +6921,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2419350</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7703D4FB-78A7-410B-93F2-2B69F189E556}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4268,11 +6977,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="results-household_power_consumption_VerySmall.txt" connectionId="2" xr16:uid="{00000000-0016-0000-0200-000005000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="results-household_power_consumption_VerySmall_1" connectionId="4" xr16:uid="{00000000-0016-0000-0200-000005000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="results-household_power_consumption_VerySmall_1" connectionId="4" xr16:uid="{00000000-0016-0000-0200-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="results-household_power_consumption_VerySmall.txt" connectionId="2" xr16:uid="{00000000-0016-0000-0200-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4541,7 +7250,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4767,7 +7476,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4776,7 +7486,7 @@
   <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="E4" activeCellId="1" sqref="A4:A14 E4:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5008,7 +7718,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E12"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>